<commit_message>
Disque lo de la hoja de vida
</commit_message>
<xml_diff>
--- a/data/datos practicantes.xlsx
+++ b/data/datos practicantes.xlsx
@@ -100,7 +100,7 @@
     <t>Aixa Ximena</t>
   </si>
   <si>
-    <t>ANDRE FERANDO</t>
+    <t>Andre Fernando</t>
   </si>
   <si>
     <t xml:space="preserve">Andrés Camilo </t>
@@ -235,7 +235,7 @@
     <t>Ramírez Mendoza</t>
   </si>
   <si>
-    <t>FLORIAN SALCEDO</t>
+    <t>Florian Salcedo</t>
   </si>
   <si>
     <t>Cala Gómez</t>
@@ -1306,7 +1306,7 @@
     <t>Jairo Contreras</t>
   </si>
   <si>
-    <t>Javier Alfonso Sarmiento Rozo</t>
+    <t>Javier</t>
   </si>
   <si>
     <t xml:space="preserve">Carolina Vargas Muñoz </t>
@@ -1675,7 +1675,7 @@
     <t xml:space="preserve">Alba Doris Morales </t>
   </si>
   <si>
-    <t>Jenny Amparo Rosales Agredo</t>
+    <t>Jenny</t>
   </si>
   <si>
     <t>Maria Camila Arango</t>
@@ -2576,12 +2576,14 @@
     <col min="13" max="13" width="32.7109375" customWidth="1"/>
     <col min="14" max="14" width="31.7109375" customWidth="1"/>
     <col min="15" max="15" width="12.7109375" customWidth="1"/>
-    <col min="16" max="17" width="47.7109375" customWidth="1"/>
+    <col min="16" max="16" width="47.7109375" customWidth="1"/>
+    <col min="17" max="17" width="47.7109375" customWidth="1"/>
     <col min="18" max="18" width="34.7109375" customWidth="1"/>
     <col min="19" max="19" width="38.7109375" customWidth="1"/>
     <col min="20" max="20" width="21.7109375" customWidth="1"/>
     <col min="21" max="21" width="14.7109375" customWidth="1"/>
-    <col min="22" max="23" width="29.7109375" customWidth="1"/>
+    <col min="22" max="22" width="29.7109375" customWidth="1"/>
+    <col min="23" max="23" width="29.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23">

</xml_diff>

<commit_message>
Correccion bug subir plan de desarrollo
</commit_message>
<xml_diff>
--- a/data/datos practicantes.xlsx
+++ b/data/datos practicantes.xlsx
@@ -1306,7 +1306,7 @@
     <t>Jairo Contreras</t>
   </si>
   <si>
-    <t>Javier</t>
+    <t>Javier Sarmiento</t>
   </si>
   <si>
     <t xml:space="preserve">Carolina Vargas Muñoz </t>
@@ -1672,7 +1672,7 @@
     <t xml:space="preserve">Alba Doris Morales </t>
   </si>
   <si>
-    <t>Jenny</t>
+    <t>Jenny Rosales</t>
   </si>
   <si>
     <t>Maria Camila Arango</t>

</xml_diff>